<commit_message>
add hex_oct converter in C
</commit_message>
<xml_diff>
--- a/WCY19XQ4_KRUKOWSKI_JAKUB.xlsx
+++ b/WCY19XQ4_KRUKOWSKI_JAKUB.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\48502\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\48502\Desktop\Wat-WDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D4D01BB-4053-4B1D-AA38-6D5E40E6BA35}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109BE329-48A1-45CC-B11D-AE1E6C94DB60}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C1A6D319-5ACF-486F-93E4-71AE9562F6F4}"/>
   </bookViews>
@@ -2799,10 +2799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{889557D9-D6BF-4FA1-992C-DDF2D68748D7}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:AE51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="V23" sqref="V23"/>
+      <selection activeCell="AB15" sqref="AB15:AE51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2814,7 +2814,7 @@
     <col min="9" max="9" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2827,7 +2827,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2836,7 +2836,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -2844,8 +2844,20 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+      <c r="W3">
+        <v>3</v>
+      </c>
+      <c r="X3">
+        <v>0.3</v>
+      </c>
+      <c r="Y3">
+        <v>0.09</v>
+      </c>
+      <c r="Z3">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2870,8 +2882,20 @@
       <c r="I4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W4">
+        <v>4</v>
+      </c>
+      <c r="X4">
+        <v>0.49</v>
+      </c>
+      <c r="Y4">
+        <v>0.13</v>
+      </c>
+      <c r="Z4">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2896,8 +2920,20 @@
       <c r="I5">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W5">
+        <v>5</v>
+      </c>
+      <c r="X5">
+        <v>0.69</v>
+      </c>
+      <c r="Y5">
+        <v>0.16</v>
+      </c>
+      <c r="Z5">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2922,8 +2958,20 @@
       <c r="I6">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W6">
+        <v>6</v>
+      </c>
+      <c r="X6">
+        <v>0.98</v>
+      </c>
+      <c r="Y6">
+        <v>0.2</v>
+      </c>
+      <c r="Z6">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2948,8 +2996,20 @@
       <c r="I7">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W7">
+        <v>7</v>
+      </c>
+      <c r="X7">
+        <v>1.26</v>
+      </c>
+      <c r="Y7">
+        <v>0.23</v>
+      </c>
+      <c r="Z7">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2974,8 +3034,20 @@
       <c r="I8">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W8">
+        <v>8</v>
+      </c>
+      <c r="X8">
+        <v>1.54</v>
+      </c>
+      <c r="Y8">
+        <v>0.26</v>
+      </c>
+      <c r="Z8">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5</v>
       </c>
@@ -3000,8 +3072,20 @@
       <c r="I9">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W9">
+        <v>9</v>
+      </c>
+      <c r="X9">
+        <v>1.82</v>
+      </c>
+      <c r="Y9">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Z9">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
@@ -3026,8 +3110,20 @@
       <c r="I10">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W10">
+        <v>10</v>
+      </c>
+      <c r="X10">
+        <v>2.1</v>
+      </c>
+      <c r="Y10">
+        <v>0.3</v>
+      </c>
+      <c r="Z10">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>7</v>
       </c>
@@ -3052,8 +3148,20 @@
       <c r="I11">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W11">
+        <v>11</v>
+      </c>
+      <c r="X11">
+        <v>2.46</v>
+      </c>
+      <c r="Y11">
+        <v>0.32</v>
+      </c>
+      <c r="Z11">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3078,8 +3186,20 @@
       <c r="I12">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W12">
+        <v>12</v>
+      </c>
+      <c r="X12">
+        <v>2.74</v>
+      </c>
+      <c r="Y12">
+        <v>0.33</v>
+      </c>
+      <c r="Z12">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>9</v>
       </c>
@@ -3104,8 +3224,20 @@
       <c r="I13">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W13">
+        <v>13</v>
+      </c>
+      <c r="X13">
+        <v>3.01</v>
+      </c>
+      <c r="Y13">
+        <v>0.35</v>
+      </c>
+      <c r="Z13">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10</v>
       </c>
@@ -3130,8 +3262,20 @@
       <c r="I14">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W14">
+        <v>14</v>
+      </c>
+      <c r="X14">
+        <v>3.37</v>
+      </c>
+      <c r="Y14">
+        <v>0.37</v>
+      </c>
+      <c r="Z14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>11</v>
       </c>
@@ -3156,8 +3300,32 @@
       <c r="I15">
         <v>0.71</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W15">
+        <v>15</v>
+      </c>
+      <c r="X15">
+        <v>3.73</v>
+      </c>
+      <c r="Y15">
+        <v>0.38</v>
+      </c>
+      <c r="Z15">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="AB15">
+        <v>3</v>
+      </c>
+      <c r="AC15">
+        <v>0.3</v>
+      </c>
+      <c r="AD15">
+        <v>0.09</v>
+      </c>
+      <c r="AE15">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>12</v>
       </c>
@@ -3182,8 +3350,32 @@
       <c r="I16">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W16">
+        <v>16</v>
+      </c>
+      <c r="X16">
+        <v>4</v>
+      </c>
+      <c r="Y16">
+        <v>0.39</v>
+      </c>
+      <c r="Z16">
+        <v>1.2</v>
+      </c>
+      <c r="AB16">
+        <v>4</v>
+      </c>
+      <c r="AC16">
+        <v>0.49</v>
+      </c>
+      <c r="AD16">
+        <v>0.13</v>
+      </c>
+      <c r="AE16">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>13</v>
       </c>
@@ -3208,8 +3400,32 @@
       <c r="I17">
         <v>0.89</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W17">
+        <v>17</v>
+      </c>
+      <c r="X17">
+        <v>4.28</v>
+      </c>
+      <c r="Y17">
+        <v>0.4</v>
+      </c>
+      <c r="Z17">
+        <v>1.29</v>
+      </c>
+      <c r="AB17">
+        <v>5</v>
+      </c>
+      <c r="AC17">
+        <v>0.69</v>
+      </c>
+      <c r="AD17">
+        <v>0.16</v>
+      </c>
+      <c r="AE17">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>14</v>
       </c>
@@ -3234,8 +3450,32 @@
       <c r="I18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W18">
+        <v>18</v>
+      </c>
+      <c r="X18">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="Y18">
+        <v>0.42</v>
+      </c>
+      <c r="Z18">
+        <v>1.41</v>
+      </c>
+      <c r="AB18">
+        <v>6</v>
+      </c>
+      <c r="AC18">
+        <v>0.98</v>
+      </c>
+      <c r="AD18">
+        <v>0.2</v>
+      </c>
+      <c r="AE18">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>15</v>
       </c>
@@ -3260,8 +3500,32 @@
       <c r="I19">
         <v>1.1200000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W19">
+        <v>19</v>
+      </c>
+      <c r="X19">
+        <v>4.93</v>
+      </c>
+      <c r="Y19">
+        <v>0.43</v>
+      </c>
+      <c r="Z19">
+        <v>1.5</v>
+      </c>
+      <c r="AB19">
+        <v>7</v>
+      </c>
+      <c r="AC19">
+        <v>1.26</v>
+      </c>
+      <c r="AD19">
+        <v>0.23</v>
+      </c>
+      <c r="AE19">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>16</v>
       </c>
@@ -3286,8 +3550,32 @@
       <c r="I20">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W20">
+        <v>20</v>
+      </c>
+      <c r="X20">
+        <v>5.3</v>
+      </c>
+      <c r="Y20">
+        <v>0.44</v>
+      </c>
+      <c r="Z20">
+        <v>1.62</v>
+      </c>
+      <c r="AB20">
+        <v>8</v>
+      </c>
+      <c r="AC20">
+        <v>1.54</v>
+      </c>
+      <c r="AD20">
+        <v>0.26</v>
+      </c>
+      <c r="AE20">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>17</v>
       </c>
@@ -3312,8 +3600,32 @@
       <c r="I21">
         <v>1.29</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W21">
+        <v>21</v>
+      </c>
+      <c r="X21">
+        <v>5.59</v>
+      </c>
+      <c r="Y21">
+        <v>0.45</v>
+      </c>
+      <c r="Z21">
+        <v>1.71</v>
+      </c>
+      <c r="AB21">
+        <v>9</v>
+      </c>
+      <c r="AC21">
+        <v>1.82</v>
+      </c>
+      <c r="AD21">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AE21">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>18</v>
       </c>
@@ -3338,8 +3650,32 @@
       <c r="I22">
         <v>1.41</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W22">
+        <v>22</v>
+      </c>
+      <c r="X22">
+        <v>5.98</v>
+      </c>
+      <c r="Y22">
+        <v>0.47</v>
+      </c>
+      <c r="Z22">
+        <v>1.84</v>
+      </c>
+      <c r="AB22">
+        <v>10</v>
+      </c>
+      <c r="AC22">
+        <v>2.1</v>
+      </c>
+      <c r="AD22">
+        <v>0.3</v>
+      </c>
+      <c r="AE22">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>19</v>
       </c>
@@ -3364,8 +3700,32 @@
       <c r="I23">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W23">
+        <v>23</v>
+      </c>
+      <c r="X23">
+        <v>6.37</v>
+      </c>
+      <c r="Y23">
+        <v>0.48</v>
+      </c>
+      <c r="Z23">
+        <v>1.96</v>
+      </c>
+      <c r="AB23">
+        <v>11</v>
+      </c>
+      <c r="AC23">
+        <v>2.46</v>
+      </c>
+      <c r="AD23">
+        <v>0.32</v>
+      </c>
+      <c r="AE23">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>20</v>
       </c>
@@ -3390,8 +3750,32 @@
       <c r="I24">
         <v>1.62</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W24">
+        <v>24</v>
+      </c>
+      <c r="X24">
+        <v>6.68</v>
+      </c>
+      <c r="Y24">
+        <v>0.49</v>
+      </c>
+      <c r="Z24">
+        <v>2.06</v>
+      </c>
+      <c r="AB24">
+        <v>12</v>
+      </c>
+      <c r="AC24">
+        <v>2.74</v>
+      </c>
+      <c r="AD24">
+        <v>0.33</v>
+      </c>
+      <c r="AE24">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>21</v>
       </c>
@@ -3416,8 +3800,32 @@
       <c r="I25">
         <v>1.71</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W25">
+        <v>25</v>
+      </c>
+      <c r="X25">
+        <v>6.98</v>
+      </c>
+      <c r="Y25">
+        <v>0.5</v>
+      </c>
+      <c r="Z25">
+        <v>2.16</v>
+      </c>
+      <c r="AB25">
+        <v>13</v>
+      </c>
+      <c r="AC25">
+        <v>3.01</v>
+      </c>
+      <c r="AD25">
+        <v>0.35</v>
+      </c>
+      <c r="AE25">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>22</v>
       </c>
@@ -3442,8 +3850,32 @@
       <c r="I26">
         <v>1.84</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W26">
+        <v>26</v>
+      </c>
+      <c r="X26">
+        <v>7.3</v>
+      </c>
+      <c r="Y26">
+        <v>0.51</v>
+      </c>
+      <c r="Z26">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="AB26">
+        <v>14</v>
+      </c>
+      <c r="AC26">
+        <v>3.37</v>
+      </c>
+      <c r="AD26">
+        <v>0.37</v>
+      </c>
+      <c r="AE26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>23</v>
       </c>
@@ -3468,8 +3900,32 @@
       <c r="I27">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W27">
+        <v>27</v>
+      </c>
+      <c r="X27">
+        <v>7.73</v>
+      </c>
+      <c r="Y27">
+        <v>0.52</v>
+      </c>
+      <c r="Z27">
+        <v>2.4</v>
+      </c>
+      <c r="AB27">
+        <v>15</v>
+      </c>
+      <c r="AC27">
+        <v>3.73</v>
+      </c>
+      <c r="AD27">
+        <v>0.38</v>
+      </c>
+      <c r="AE27">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>24</v>
       </c>
@@ -3494,8 +3950,32 @@
       <c r="I28">
         <v>2.06</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W28">
+        <v>28</v>
+      </c>
+      <c r="X28">
+        <v>8.06</v>
+      </c>
+      <c r="Y28">
+        <v>0.53</v>
+      </c>
+      <c r="Z28">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="AB28">
+        <v>16</v>
+      </c>
+      <c r="AC28">
+        <v>4</v>
+      </c>
+      <c r="AD28">
+        <v>0.39</v>
+      </c>
+      <c r="AE28">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>25</v>
       </c>
@@ -3520,8 +4000,32 @@
       <c r="I29">
         <v>2.16</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W29">
+        <v>29</v>
+      </c>
+      <c r="X29">
+        <v>8.4</v>
+      </c>
+      <c r="Y29">
+        <v>0.54</v>
+      </c>
+      <c r="Z29">
+        <v>2.62</v>
+      </c>
+      <c r="AB29">
+        <v>17</v>
+      </c>
+      <c r="AC29">
+        <v>4.28</v>
+      </c>
+      <c r="AD29">
+        <v>0.4</v>
+      </c>
+      <c r="AE29">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>26</v>
       </c>
@@ -3546,8 +4050,32 @@
       <c r="I30">
         <v>2.2599999999999998</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W30">
+        <v>30</v>
+      </c>
+      <c r="X30">
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="Y30">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="Z30">
+        <v>2.77</v>
+      </c>
+      <c r="AB30">
+        <v>18</v>
+      </c>
+      <c r="AC30">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="AD30">
+        <v>0.42</v>
+      </c>
+      <c r="AE30">
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>27</v>
       </c>
@@ -3572,8 +4100,32 @@
       <c r="I31">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W31">
+        <v>31</v>
+      </c>
+      <c r="X31">
+        <v>9.24</v>
+      </c>
+      <c r="Y31">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Z31">
+        <v>2.89</v>
+      </c>
+      <c r="AB31">
+        <v>19</v>
+      </c>
+      <c r="AC31">
+        <v>4.93</v>
+      </c>
+      <c r="AD31">
+        <v>0.43</v>
+      </c>
+      <c r="AE31">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>28</v>
       </c>
@@ -3598,8 +4150,32 @@
       <c r="I32">
         <v>2.5099999999999998</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W32">
+        <v>32</v>
+      </c>
+      <c r="X32">
+        <v>9.61</v>
+      </c>
+      <c r="Y32">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Z32">
+        <v>3.01</v>
+      </c>
+      <c r="AB32">
+        <v>20</v>
+      </c>
+      <c r="AC32">
+        <v>5.3</v>
+      </c>
+      <c r="AD32">
+        <v>0.44</v>
+      </c>
+      <c r="AE32">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>29</v>
       </c>
@@ -3624,8 +4200,32 @@
       <c r="I33">
         <v>2.62</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W33">
+        <v>33</v>
+      </c>
+      <c r="X33">
+        <v>10</v>
+      </c>
+      <c r="Y33">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="Z33">
+        <v>3.14</v>
+      </c>
+      <c r="AB33">
+        <v>21</v>
+      </c>
+      <c r="AC33">
+        <v>5.59</v>
+      </c>
+      <c r="AD33">
+        <v>0.45</v>
+      </c>
+      <c r="AE33">
+        <v>1.71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>30</v>
       </c>
@@ -3650,8 +4250,32 @@
       <c r="I34">
         <v>2.77</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W34">
+        <v>34</v>
+      </c>
+      <c r="X34">
+        <v>11.3</v>
+      </c>
+      <c r="Y34">
+        <v>0.61</v>
+      </c>
+      <c r="Z34">
+        <v>3.55</v>
+      </c>
+      <c r="AB34">
+        <v>22</v>
+      </c>
+      <c r="AC34">
+        <v>5.98</v>
+      </c>
+      <c r="AD34">
+        <v>0.47</v>
+      </c>
+      <c r="AE34">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>31</v>
       </c>
@@ -3676,8 +4300,32 @@
       <c r="I35">
         <v>2.89</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W35">
+        <v>35</v>
+      </c>
+      <c r="X35">
+        <v>12.4</v>
+      </c>
+      <c r="Y35">
+        <v>0.64</v>
+      </c>
+      <c r="Z35">
+        <v>3.93</v>
+      </c>
+      <c r="AB35">
+        <v>23</v>
+      </c>
+      <c r="AC35">
+        <v>6.37</v>
+      </c>
+      <c r="AD35">
+        <v>0.48</v>
+      </c>
+      <c r="AE35">
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>32</v>
       </c>
@@ -3702,8 +4350,32 @@
       <c r="I36">
         <v>3.01</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W36">
+        <v>36</v>
+      </c>
+      <c r="X36">
+        <v>13.3</v>
+      </c>
+      <c r="Y36">
+        <v>0.66</v>
+      </c>
+      <c r="Z36">
+        <v>4.22</v>
+      </c>
+      <c r="AB36">
+        <v>24</v>
+      </c>
+      <c r="AC36">
+        <v>6.68</v>
+      </c>
+      <c r="AD36">
+        <v>0.49</v>
+      </c>
+      <c r="AE36">
+        <v>2.06</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>33</v>
       </c>
@@ -3728,8 +4400,32 @@
       <c r="I37">
         <v>3.14</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W37">
+        <v>37</v>
+      </c>
+      <c r="X37">
+        <v>14.2</v>
+      </c>
+      <c r="Y37">
+        <v>0.68</v>
+      </c>
+      <c r="Z37">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="AB37">
+        <v>25</v>
+      </c>
+      <c r="AC37">
+        <v>6.98</v>
+      </c>
+      <c r="AD37">
+        <v>0.5</v>
+      </c>
+      <c r="AE37">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
       <c r="F38">
         <v>34</v>
       </c>
@@ -3742,8 +4438,32 @@
       <c r="I38">
         <v>3.55</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W38">
+        <v>38</v>
+      </c>
+      <c r="X38">
+        <v>15</v>
+      </c>
+      <c r="Y38">
+        <v>0.69</v>
+      </c>
+      <c r="Z38">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="AB38">
+        <v>26</v>
+      </c>
+      <c r="AC38">
+        <v>7.3</v>
+      </c>
+      <c r="AD38">
+        <v>0.51</v>
+      </c>
+      <c r="AE38">
+        <v>2.2599999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
       <c r="F39">
         <v>35</v>
       </c>
@@ -3756,8 +4476,32 @@
       <c r="I39">
         <v>3.93</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="W39">
+        <v>39</v>
+      </c>
+      <c r="X39">
+        <v>16.3</v>
+      </c>
+      <c r="Y39">
+        <v>0.72</v>
+      </c>
+      <c r="Z39">
+        <v>5.21</v>
+      </c>
+      <c r="AB39">
+        <v>27</v>
+      </c>
+      <c r="AC39">
+        <v>7.73</v>
+      </c>
+      <c r="AD39">
+        <v>0.52</v>
+      </c>
+      <c r="AE39">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
       <c r="F40">
         <v>36</v>
       </c>
@@ -3770,8 +4514,20 @@
       <c r="I40">
         <v>4.22</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="AB40">
+        <v>28</v>
+      </c>
+      <c r="AC40">
+        <v>8.06</v>
+      </c>
+      <c r="AD40">
+        <v>0.53</v>
+      </c>
+      <c r="AE40">
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
       <c r="F41">
         <v>37</v>
       </c>
@@ -3784,8 +4540,20 @@
       <c r="I41">
         <v>4.5199999999999996</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="AB41">
+        <v>29</v>
+      </c>
+      <c r="AC41">
+        <v>8.4</v>
+      </c>
+      <c r="AD41">
+        <v>0.54</v>
+      </c>
+      <c r="AE41">
+        <v>2.62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
       <c r="F42">
         <v>38</v>
       </c>
@@ -3798,8 +4566,20 @@
       <c r="I42">
         <v>4.7699999999999996</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="AB42">
+        <v>30</v>
+      </c>
+      <c r="AC42">
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="AD42">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AE42">
+        <v>2.77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
       <c r="F43">
         <v>39</v>
       </c>
@@ -3812,8 +4592,20 @@
       <c r="I43">
         <v>5.21</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="AB43">
+        <v>31</v>
+      </c>
+      <c r="AC43">
+        <v>9.24</v>
+      </c>
+      <c r="AD43">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="AE43">
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
       <c r="F44">
         <v>40</v>
       </c>
@@ -3826,8 +4618,20 @@
       <c r="I44">
         <v>5.82</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="AB44">
+        <v>32</v>
+      </c>
+      <c r="AC44">
+        <v>9.61</v>
+      </c>
+      <c r="AD44">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AE44">
+        <v>3.01</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
       <c r="F45">
         <v>41</v>
       </c>
@@ -3839,6 +4643,102 @@
       </c>
       <c r="I45">
         <v>6.4</v>
+      </c>
+      <c r="AB45">
+        <v>33</v>
+      </c>
+      <c r="AC45">
+        <v>10</v>
+      </c>
+      <c r="AD45">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AE45">
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AB46">
+        <v>34</v>
+      </c>
+      <c r="AC46">
+        <v>11.3</v>
+      </c>
+      <c r="AD46">
+        <v>0.61</v>
+      </c>
+      <c r="AE46">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AB47">
+        <v>35</v>
+      </c>
+      <c r="AC47">
+        <v>12.4</v>
+      </c>
+      <c r="AD47">
+        <v>0.64</v>
+      </c>
+      <c r="AE47">
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AB48">
+        <v>36</v>
+      </c>
+      <c r="AC48">
+        <v>13.3</v>
+      </c>
+      <c r="AD48">
+        <v>0.66</v>
+      </c>
+      <c r="AE48">
+        <v>4.22</v>
+      </c>
+    </row>
+    <row r="49" spans="28:31" x14ac:dyDescent="0.3">
+      <c r="AB49">
+        <v>37</v>
+      </c>
+      <c r="AC49">
+        <v>14.2</v>
+      </c>
+      <c r="AD49">
+        <v>0.68</v>
+      </c>
+      <c r="AE49">
+        <v>4.5199999999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="28:31" x14ac:dyDescent="0.3">
+      <c r="AB50">
+        <v>38</v>
+      </c>
+      <c r="AC50">
+        <v>15</v>
+      </c>
+      <c r="AD50">
+        <v>0.69</v>
+      </c>
+      <c r="AE50">
+        <v>4.7699999999999996</v>
+      </c>
+    </row>
+    <row r="51" spans="28:31" x14ac:dyDescent="0.3">
+      <c r="AB51">
+        <v>39</v>
+      </c>
+      <c r="AC51">
+        <v>16.3</v>
+      </c>
+      <c r="AD51">
+        <v>0.72</v>
+      </c>
+      <c r="AE51">
+        <v>5.21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>